<commit_message>
Reconfigurable Robot Navigation - All environments and results
</commit_message>
<xml_diff>
--- a/00_Final/Results/Slit.xlsx
+++ b/00_Final/Results/Slit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pppp8\Documents\HTo_GA\00_Final\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA29816-E9B9-45FF-8D99-AB82376B48EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F442432A-C46C-45BB-A1AD-4DAA1D2B91DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1200" windowWidth="26685" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GAresult0" sheetId="1" r:id="rId1"/>
@@ -4978,8 +4978,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7657370953630798E-2"/>
-          <c:y val="3.510879874102818E-2"/>
+          <c:x val="8.5788906473004065E-2"/>
+          <c:y val="2.1754071606433813E-2"/>
           <c:w val="0.8859537401574803"/>
           <c:h val="0.82292573795484447"/>
         </c:manualLayout>
@@ -10220,16 +10220,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>105062</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>56000</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>281955</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>65</xdr:col>
-      <xdr:colOff>172989</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>48380</xdr:rowOff>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>349882</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>34771</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10844,8 +10844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BU18" sqref="BU18"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BR12" sqref="BR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>